<commit_message>
Append to Report-2025-05-01.xlsx at ٠١‏/٠٥‏/٢٠٢٥ ٠٤:٠٨:٠٩ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -454,9 +454,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٠٤:٤٢ م</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v/>
+      </c>
+      <c r="B3" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C3" t="str">
+        <v>2323</v>
+      </c>
+      <c r="D3" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E3" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F3" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G3" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H3" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٠٨:٠٩ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-01.xlsx at ٠١‏/٠٥‏/٢٠٢٥ ٠٤:٢١:٢٢ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -480,9 +480,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٠٨:٠٩ م</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>222</v>
+      </c>
+      <c r="B4" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C4" t="str">
+        <v>2000</v>
+      </c>
+      <c r="D4" t="str">
+        <v>الجزائري</v>
+      </c>
+      <c r="E4" t="str">
+        <v>الرحلة 1</v>
+      </c>
+      <c r="F4" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G4" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H4" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٢١:٢٢ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-01.xlsx at ٠١‏/٠٥‏/٢٠٢٥ ٠٤:٢٩:٣٠ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -506,9 +506,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٢١:٢٢ م</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v/>
+      </c>
+      <c r="B5" t="str">
+        <v xml:space="preserve">حسن </v>
+      </c>
+      <c r="C5" t="str">
+        <v>200</v>
+      </c>
+      <c r="D5" t="str">
+        <v>النصر</v>
+      </c>
+      <c r="E5" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="F5" t="str">
+        <v>C4</v>
+      </c>
+      <c r="G5" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H5" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٢٩:٣٠ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-01.xlsx at ٠١‏/٠٥‏/٢٠٢٥ ٠٤:٣٧:١٠ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -532,9 +532,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٢٩:٣٠ م</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v/>
+      </c>
+      <c r="B6" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C6" t="str">
+        <v>22</v>
+      </c>
+      <c r="D6" t="str">
+        <v>الجزائري</v>
+      </c>
+      <c r="E6" t="str">
+        <v>الرحلة 1</v>
+      </c>
+      <c r="F6" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G6" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H6" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٣٧:١٠ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-01.xlsx at ٠١‏/٠٥‏/٢٠٢٥ ٠٤:٣٨:١١ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -558,9 +558,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٣٧:١٠ م</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v/>
+      </c>
+      <c r="B7" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C7" t="str">
+        <v>22</v>
+      </c>
+      <c r="D7" t="str">
+        <v>الجزائري</v>
+      </c>
+      <c r="E7" t="str">
+        <v>الرحلة 1</v>
+      </c>
+      <c r="F7" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G7" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H7" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٣٨:١١ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-01.xlsx at ٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٠:٠٤ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -584,9 +584,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٣٨:١١ م</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v/>
+      </c>
+      <c r="B8" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C8" t="str">
+        <v>22</v>
+      </c>
+      <c r="D8" t="str">
+        <v>الجزائري</v>
+      </c>
+      <c r="E8" t="str">
+        <v>الرحلة 1</v>
+      </c>
+      <c r="F8" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G8" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H8" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٠:٠٤ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-01.xlsx at ٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤١:٠٤ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -610,9 +610,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٠:٠٤ م</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v/>
+      </c>
+      <c r="B9" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C9" t="str">
+        <v>6</v>
+      </c>
+      <c r="D9" t="str">
+        <v>الجزائري</v>
+      </c>
+      <c r="E9" t="str">
+        <v>الرحلة 1</v>
+      </c>
+      <c r="F9" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G9" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H9" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤١:٠٤ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-01.xlsx at ٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٢:٠٤ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -636,9 +636,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤١:٠٤ م</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v/>
+      </c>
+      <c r="B10" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C10" t="str">
+        <v>2</v>
+      </c>
+      <c r="D10" t="str">
+        <v>الجزائري</v>
+      </c>
+      <c r="E10" t="str">
+        <v>الرحلة 1</v>
+      </c>
+      <c r="F10" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G10" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H10" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٢:٠٤ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-01.xlsx at ٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٤:٥٣ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -662,9 +662,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٢:٠٤ م</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v/>
+      </c>
+      <c r="B11" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C11" t="str">
+        <v>33</v>
+      </c>
+      <c r="D11" t="str">
+        <v>الجزائري</v>
+      </c>
+      <c r="E11" t="str">
+        <v>الرحلة 1</v>
+      </c>
+      <c r="F11" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G11" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H11" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٤:٥٣ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 50 rows at 2025-05-01T13:48:32.320Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -792,9 +792,1309 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٦:٢١ م</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v/>
+      </c>
+      <c r="B16" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C16" t="str">
+        <v>2222</v>
+      </c>
+      <c r="D16" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E16" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F16" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G16" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H16" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v/>
+      </c>
+      <c r="B17" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C17" t="str">
+        <v>22</v>
+      </c>
+      <c r="D17" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E17" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F17" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G17" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H17" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v/>
+      </c>
+      <c r="B18" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C18" t="str">
+        <v>1</v>
+      </c>
+      <c r="D18" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E18" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F18" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G18" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H18" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v/>
+      </c>
+      <c r="B19" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C19" t="str">
+        <v>0</v>
+      </c>
+      <c r="D19" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E19" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F19" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G19" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H19" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v/>
+      </c>
+      <c r="B20" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C20" t="str">
+        <v>123</v>
+      </c>
+      <c r="D20" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E20" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F20" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G20" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H20" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v/>
+      </c>
+      <c r="B21" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C21" t="str">
+        <v>44</v>
+      </c>
+      <c r="D21" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E21" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F21" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G21" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H21" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v/>
+      </c>
+      <c r="B22" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C22" t="str">
+        <v>11</v>
+      </c>
+      <c r="D22" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E22" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F22" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G22" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H22" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v/>
+      </c>
+      <c r="B23" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C23" t="str">
+        <v>121212</v>
+      </c>
+      <c r="D23" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E23" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F23" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G23" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H23" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v/>
+      </c>
+      <c r="B24" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C24" t="str">
+        <v>2323</v>
+      </c>
+      <c r="D24" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E24" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F24" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G24" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H24" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v/>
+      </c>
+      <c r="B25" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C25" t="str">
+        <v>11212</v>
+      </c>
+      <c r="D25" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E25" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F25" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G25" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H25" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v/>
+      </c>
+      <c r="B26" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C26" t="str">
+        <v>232323</v>
+      </c>
+      <c r="D26" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E26" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F26" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G26" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H26" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v/>
+      </c>
+      <c r="B27" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C27" t="str">
+        <v>12312</v>
+      </c>
+      <c r="D27" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E27" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F27" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G27" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H27" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v/>
+      </c>
+      <c r="B28" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C28" t="str">
+        <v>123123</v>
+      </c>
+      <c r="D28" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E28" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F28" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G28" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H28" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v/>
+      </c>
+      <c r="B29" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C29" t="str">
+        <v>123123</v>
+      </c>
+      <c r="D29" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E29" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F29" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G29" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H29" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v/>
+      </c>
+      <c r="B30" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C30" t="str">
+        <v>123123</v>
+      </c>
+      <c r="D30" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E30" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F30" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G30" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H30" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v/>
+      </c>
+      <c r="B31" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C31" t="str">
+        <v>123123</v>
+      </c>
+      <c r="D31" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E31" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F31" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G31" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H31" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v/>
+      </c>
+      <c r="B32" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C32" t="str">
+        <v>12123123</v>
+      </c>
+      <c r="D32" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E32" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F32" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G32" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H32" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v/>
+      </c>
+      <c r="B33" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C33" t="str">
+        <v>12132123</v>
+      </c>
+      <c r="D33" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E33" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F33" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G33" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H33" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v/>
+      </c>
+      <c r="B34" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C34" t="str">
+        <v>123123123</v>
+      </c>
+      <c r="D34" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E34" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F34" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G34" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H34" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v/>
+      </c>
+      <c r="B35" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C35" t="str">
+        <v>123123123</v>
+      </c>
+      <c r="D35" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E35" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F35" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G35" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H35" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v/>
+      </c>
+      <c r="B36" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C36" t="str">
+        <v>123123</v>
+      </c>
+      <c r="D36" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E36" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F36" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G36" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H36" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v/>
+      </c>
+      <c r="B37" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C37" t="str">
+        <v>123123</v>
+      </c>
+      <c r="D37" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E37" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F37" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G37" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H37" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v/>
+      </c>
+      <c r="B38" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C38" t="str">
+        <v>12123123</v>
+      </c>
+      <c r="D38" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E38" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F38" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G38" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H38" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v/>
+      </c>
+      <c r="B39" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C39" t="str">
+        <v>123123</v>
+      </c>
+      <c r="D39" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E39" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F39" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G39" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H39" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v/>
+      </c>
+      <c r="B40" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C40" t="str">
+        <v>123123123</v>
+      </c>
+      <c r="D40" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E40" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F40" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G40" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H40" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v/>
+      </c>
+      <c r="B41" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C41" t="str">
+        <v>12123123</v>
+      </c>
+      <c r="D41" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E41" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F41" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G41" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H41" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v/>
+      </c>
+      <c r="B42" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C42" t="str">
+        <v>123123123</v>
+      </c>
+      <c r="D42" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E42" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F42" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G42" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H42" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v/>
+      </c>
+      <c r="B43" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C43" t="str">
+        <v>12313123</v>
+      </c>
+      <c r="D43" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E43" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F43" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G43" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H43" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v/>
+      </c>
+      <c r="B44" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C44" t="str">
+        <v>123123123</v>
+      </c>
+      <c r="D44" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E44" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F44" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G44" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H44" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v/>
+      </c>
+      <c r="B45" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C45" t="str">
+        <v>123123</v>
+      </c>
+      <c r="D45" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E45" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F45" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G45" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H45" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v/>
+      </c>
+      <c r="B46" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C46" t="str">
+        <v>112323</v>
+      </c>
+      <c r="D46" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E46" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F46" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G46" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H46" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v/>
+      </c>
+      <c r="B47" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C47" t="str">
+        <v>121231233</v>
+      </c>
+      <c r="D47" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E47" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F47" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G47" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H47" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v/>
+      </c>
+      <c r="B48" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C48" t="str">
+        <v>123</v>
+      </c>
+      <c r="D48" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E48" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F48" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G48" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H48" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v/>
+      </c>
+      <c r="B49" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C49" t="str">
+        <v>123123</v>
+      </c>
+      <c r="D49" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E49" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F49" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G49" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H49" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v/>
+      </c>
+      <c r="B50" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C50" t="str">
+        <v>123123</v>
+      </c>
+      <c r="D50" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E50" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F50" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G50" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H50" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v/>
+      </c>
+      <c r="B51" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C51" t="str">
+        <v>1</v>
+      </c>
+      <c r="D51" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E51" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F51" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G51" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H51" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v/>
+      </c>
+      <c r="B52" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C52" t="str">
+        <v>1</v>
+      </c>
+      <c r="D52" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E52" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F52" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G52" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H52" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v/>
+      </c>
+      <c r="B53" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C53" t="str">
+        <v>1</v>
+      </c>
+      <c r="D53" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E53" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F53" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G53" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H53" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v/>
+      </c>
+      <c r="B54" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C54" t="str">
+        <v>1</v>
+      </c>
+      <c r="D54" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E54" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F54" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G54" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H54" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v/>
+      </c>
+      <c r="B55" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C55" t="str">
+        <v>1</v>
+      </c>
+      <c r="D55" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E55" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F55" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G55" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H55" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v/>
+      </c>
+      <c r="B56" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C56" t="str">
+        <v>2</v>
+      </c>
+      <c r="D56" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E56" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F56" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G56" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H56" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v/>
+      </c>
+      <c r="B57" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C57" t="str">
+        <v>2</v>
+      </c>
+      <c r="D57" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E57" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F57" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G57" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H57" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v/>
+      </c>
+      <c r="B58" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C58" t="str">
+        <v>1</v>
+      </c>
+      <c r="D58" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E58" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F58" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G58" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H58" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v/>
+      </c>
+      <c r="B59" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C59" t="str">
+        <v>1</v>
+      </c>
+      <c r="D59" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E59" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F59" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G59" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H59" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v/>
+      </c>
+      <c r="B60" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C60" t="str">
+        <v>2</v>
+      </c>
+      <c r="D60" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E60" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F60" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G60" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H60" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v/>
+      </c>
+      <c r="B61" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C61" t="str">
+        <v>2</v>
+      </c>
+      <c r="D61" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E61" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F61" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G61" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H61" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v/>
+      </c>
+      <c r="B62" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C62" t="str">
+        <v>2</v>
+      </c>
+      <c r="D62" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E62" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F62" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G62" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H62" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v/>
+      </c>
+      <c r="B63" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C63" t="str">
+        <v>3</v>
+      </c>
+      <c r="D63" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E63" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F63" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G63" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H63" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v/>
+      </c>
+      <c r="B64" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C64" t="str">
+        <v>1</v>
+      </c>
+      <c r="D64" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E64" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F64" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G64" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H64" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v/>
+      </c>
+      <c r="B65" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C65" t="str">
+        <v>1</v>
+      </c>
+      <c r="D65" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E65" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F65" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G65" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H65" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٤٨:٣٢ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H65"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 4 rows at 2025-05-01T13:55:14.588Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -818,9 +818,113 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٥١:٢٨ م</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v/>
+      </c>
+      <c r="B17" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C17" t="str">
+        <v>23</v>
+      </c>
+      <c r="D17" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E17" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="F17" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G17" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H17" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٥٥:١٤ م</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v/>
+      </c>
+      <c r="B18" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C18" t="str">
+        <v>23</v>
+      </c>
+      <c r="D18" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E18" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="F18" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G18" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H18" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٥٥:١٤ م</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>23</v>
+      </c>
+      <c r="B19" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C19" t="str">
+        <v>2323</v>
+      </c>
+      <c r="D19" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E19" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="F19" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G19" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H19" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٥٥:١٤ م</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v/>
+      </c>
+      <c r="B20" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C20" t="str">
+        <v>34</v>
+      </c>
+      <c r="D20" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E20" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="F20" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G20" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H20" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٤:٥٥:١٤ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H20"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T14:01:30.351Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1078,9 +1078,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٠١:٢٠ م</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v/>
+      </c>
+      <c r="B27" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C27" t="str">
+        <v>1</v>
+      </c>
+      <c r="D27" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E27" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="F27" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G27" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H27" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٠١:٣٠ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H26"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H27"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T14:03:52.161Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1104,9 +1104,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٠١:٣٠ م</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v/>
+      </c>
+      <c r="B28" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C28" t="str">
+        <v>22</v>
+      </c>
+      <c r="D28" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E28" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F28" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G28" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H28" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٠٣:٥٢ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H27"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H28"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T14:06:25.552Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1130,9 +1130,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٠٣:٥٢ م</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v/>
+      </c>
+      <c r="B29" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C29" t="str">
+        <v>222</v>
+      </c>
+      <c r="D29" t="str">
+        <v>النصر</v>
+      </c>
+      <c r="E29" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="F29" t="str">
+        <v>C4</v>
+      </c>
+      <c r="G29" t="str">
+        <v>IDRF</v>
+      </c>
+      <c r="H29" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٠٦:٢٥ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H28"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H29"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T14:08:19.935Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1156,9 +1156,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٠٦:٢٥ م</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v/>
+      </c>
+      <c r="B30" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C30" t="str">
+        <v>22</v>
+      </c>
+      <c r="D30" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E30" t="str">
+        <v>الرحلة 1</v>
+      </c>
+      <c r="F30" t="str">
+        <v>C1</v>
+      </c>
+      <c r="G30" t="str">
+        <v>WCK</v>
+      </c>
+      <c r="H30" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٠٨:١٩ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H29"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H30"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T14:09:56.393Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1182,9 +1182,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٠٨:١٩ م</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v/>
+      </c>
+      <c r="B31" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C31" t="str">
+        <v>22</v>
+      </c>
+      <c r="D31" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E31" t="str">
+        <v>الرحلة 1</v>
+      </c>
+      <c r="F31" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G31" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H31" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٠٩:٥٦ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H30"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H31"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T14:13:29.771Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -454,9 +454,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:١٣:٥٥ م</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v/>
+      </c>
+      <c r="B3" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C3" t="str">
+        <v>222</v>
+      </c>
+      <c r="D3" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E3" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="F3" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G3" t="str">
+        <v>WCK</v>
+      </c>
+      <c r="H3" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:١٣:٢٩ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T14:14:32.329Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -480,9 +480,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:١٣:٢٩ م</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v/>
+      </c>
+      <c r="B4" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C4" t="str">
+        <v>22</v>
+      </c>
+      <c r="D4" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E4" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="F4" t="str">
+        <v>C1</v>
+      </c>
+      <c r="G4" t="str">
+        <v>UNICEF</v>
+      </c>
+      <c r="H4" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:١٤:٣٢ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T14:15:32.401Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -506,9 +506,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:١٤:٣٢ م</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>23</v>
+      </c>
+      <c r="B5" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C5" t="str">
+        <v>234</v>
+      </c>
+      <c r="D5" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E5" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="F5" t="str">
+        <v>C1</v>
+      </c>
+      <c r="G5" t="str">
+        <v>UNICEF</v>
+      </c>
+      <c r="H5" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:١٥:٣٢ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T14:17:33.783Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -532,9 +532,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:١٥:٣٢ م</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v/>
+      </c>
+      <c r="B6" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2323</v>
+      </c>
+      <c r="D6" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E6" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F6" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G6" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H6" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:١٧:٣٣ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T14:19:45.376Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -558,9 +558,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:١٧:٣٣ م</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v/>
+      </c>
+      <c r="B7" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C7" t="str">
+        <v>2323</v>
+      </c>
+      <c r="D7" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E7" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F7" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G7" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H7" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:١٩:٤٥ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T14:20:57.245Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -584,9 +584,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:١٩:٤٥ م</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v/>
+      </c>
+      <c r="B8" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2323</v>
+      </c>
+      <c r="D8" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E8" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F8" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G8" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H8" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٢٠:٥٧ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T14:22:29.746Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -610,9 +610,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٢٠:٥٧ م</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v/>
+      </c>
+      <c r="B9" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C9" t="str">
+        <v>2323</v>
+      </c>
+      <c r="D9" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E9" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F9" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G9" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H9" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٢٢:٢٩ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T14:24:47.580Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -636,9 +636,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٢٣:٢٩ م</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v/>
+      </c>
+      <c r="B10" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C10" t="str">
+        <v>2323</v>
+      </c>
+      <c r="D10" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E10" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F10" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G10" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H10" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٢٤:٤٧ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-01.xlsx at ٠١‏/٠٥‏/٢٠٢٥ ٠٥:٣٧:٤٧ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -662,9 +662,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٢٤:٤٧ م</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v/>
+      </c>
+      <c r="B11" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C11" t="str">
+        <v>2323</v>
+      </c>
+      <c r="D11" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E11" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F11" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G11" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H11" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٣٧:٤٧ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-01.xlsx at ٠١‏/٠٥‏/٢٠٢٥ ٠٥:٥٧:٢٥ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -688,9 +688,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٣٧:٤٧ م</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v/>
+      </c>
+      <c r="B12" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C12" t="str">
+        <v>2323</v>
+      </c>
+      <c r="D12" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E12" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F12" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G12" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H12" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٥٧:٢٥ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-01.xlsx at ٠١‏/٠٥‏/٢٠٢٥ ٠٥:٥٨:٣٩ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -714,9 +714,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٥٧:٢٥ م</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v/>
+      </c>
+      <c r="B13" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C13" t="str">
+        <v>222</v>
+      </c>
+      <c r="D13" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E13" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="F13" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G13" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H13" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٥٨:٣٩ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H13"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T15:01:55.895Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -740,9 +740,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٥:٥٨:٣٩ م</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v/>
+      </c>
+      <c r="B14" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C14" t="str">
+        <v>2</v>
+      </c>
+      <c r="D14" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E14" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F14" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G14" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H14" t="str">
+        <v>٠٦:٠١:٥٥ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 2 rows at 2025-05-01T15:03:48.576Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -766,9 +766,35 @@
         <v>٠٦:٠١:٥٥ م</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v/>
+      </c>
+      <c r="B15" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C15" t="str">
+        <v>200</v>
+      </c>
+      <c r="D15" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E15" t="str">
+        <v>الرحلة 1</v>
+      </c>
+      <c r="F15" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G15" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H15" t="str">
+        <v>٠٦:٠٣:٤٨ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H15"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-01.xlsx at ٠١‏/٠٥‏/٢٠٢٥ ٠٦:١٤:٢٠ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -792,9 +792,35 @@
         <v>٠٦:٠٣:٤٨ م</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v/>
+      </c>
+      <c r="B16" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C16" t="str">
+        <v>8</v>
+      </c>
+      <c r="D16" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E16" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F16" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G16" t="str">
+        <v>IDRF</v>
+      </c>
+      <c r="H16" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:١٤:٢٠ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H16"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-01.xlsx at ٠١‏/٠٥‏/٢٠٢٥ ٠٦:١٦:٤١ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -818,9 +818,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:١٤:٢٠ م</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v/>
+      </c>
+      <c r="B17" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C17" t="str">
+        <v>2</v>
+      </c>
+      <c r="D17" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E17" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F17" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G17" t="str">
+        <v>IDRF</v>
+      </c>
+      <c r="H17" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:١٦:٤١ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-01.xlsx at ٠١‏/٠٥‏/٢٠٢٥ ٠٦:٢٢:٣٤ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -844,9 +844,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:١٦:٤١ م</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v/>
+      </c>
+      <c r="B18" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C18" t="str">
+        <v>2</v>
+      </c>
+      <c r="D18" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E18" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F18" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G18" t="str">
+        <v>IDRF</v>
+      </c>
+      <c r="H18" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٢٢:٣٤ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H18"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-01.xlsx at ٠١‏/٠٥‏/٢٠٢٥ ٠٦:٢٣:٤٥ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -870,9 +870,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٢٢:٣٤ م</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v/>
+      </c>
+      <c r="B19" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C19" t="str">
+        <v>2</v>
+      </c>
+      <c r="D19" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E19" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F19" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G19" t="str">
+        <v>IDRF</v>
+      </c>
+      <c r="H19" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٢٣:٤٥ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H19"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T15:30:00.588Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -454,9 +454,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٢٩:١١ م</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v/>
+      </c>
+      <c r="B3" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C3" t="str">
+        <v>2</v>
+      </c>
+      <c r="D3" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E3" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F3" t="str">
+        <v>C1</v>
+      </c>
+      <c r="G3" t="str">
+        <v>UNICEF</v>
+      </c>
+      <c r="H3" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٣٠:٠٠ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 2 rows at 2025-05-01T15:32:41.762Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -480,9 +480,61 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٣٠:٠٠ م</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v/>
+      </c>
+      <c r="B4" t="str">
+        <v xml:space="preserve">حسن </v>
+      </c>
+      <c r="C4" t="str">
+        <v>23</v>
+      </c>
+      <c r="D4" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E4" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F4" t="str">
+        <v>C1</v>
+      </c>
+      <c r="G4" t="str">
+        <v>UNICEF</v>
+      </c>
+      <c r="H4" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٣٢:٤١ م</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v/>
+      </c>
+      <c r="B5" t="str">
+        <v xml:space="preserve">حسن </v>
+      </c>
+      <c r="C5" t="str">
+        <v>23</v>
+      </c>
+      <c r="D5" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E5" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F5" t="str">
+        <v>C1</v>
+      </c>
+      <c r="G5" t="str">
+        <v>UNICEF</v>
+      </c>
+      <c r="H5" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٣٢:٤١ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 3 rows at 2025-05-01T15:37:39.981Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -532,9 +532,87 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٣٢:٤١ م</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v/>
+      </c>
+      <c r="B6" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2</v>
+      </c>
+      <c r="D6" t="str">
+        <v>الجزائري</v>
+      </c>
+      <c r="E6" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F6" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G6" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H6" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٣٧:٣٩ م</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>2</v>
+      </c>
+      <c r="B7" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C7" t="str">
+        <v>2</v>
+      </c>
+      <c r="D7" t="str">
+        <v>الجزائري</v>
+      </c>
+      <c r="E7" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F7" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G7" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H7" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٣٧:٣٩ م</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>2</v>
+      </c>
+      <c r="B8" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2</v>
+      </c>
+      <c r="D8" t="str">
+        <v>الجزائري</v>
+      </c>
+      <c r="E8" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F8" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G8" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H8" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٣٧:٣٩ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T15:38:55.247Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -454,9 +454,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٣٨:٤٩ م</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v/>
+      </c>
+      <c r="B3" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C3" t="str">
+        <v>500</v>
+      </c>
+      <c r="D3" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E3" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="F3" t="str">
+        <v>C5</v>
+      </c>
+      <c r="G3" t="str">
+        <v>UNICEF</v>
+      </c>
+      <c r="H3" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٣٨:٥٥ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T15:41:49.849Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -480,9 +480,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٣٨:٥٥ م</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v/>
+      </c>
+      <c r="B4" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C4" t="str">
+        <v>12</v>
+      </c>
+      <c r="D4" t="str">
+        <v>الجزائري</v>
+      </c>
+      <c r="E4" t="str">
+        <v>الرحلة 1</v>
+      </c>
+      <c r="F4" t="str">
+        <v>C1</v>
+      </c>
+      <c r="G4" t="str">
+        <v>UNICEF</v>
+      </c>
+      <c r="H4" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٤١:٤٩ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T15:42:50.875Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -506,9 +506,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٤١:٤٩ م</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v/>
+      </c>
+      <c r="B5" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C5" t="str">
+        <v>20</v>
+      </c>
+      <c r="D5" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E5" t="str">
+        <v>الرحلة 1</v>
+      </c>
+      <c r="F5" t="str">
+        <v>C1</v>
+      </c>
+      <c r="G5" t="str">
+        <v>UNICEF</v>
+      </c>
+      <c r="H5" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٤٢:٥٠ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T15:44:16.289Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -532,9 +532,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٤٢:٥٠ م</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>21</v>
+      </c>
+      <c r="B6" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C6" t="str">
+        <v>50</v>
+      </c>
+      <c r="D6" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E6" t="str">
+        <v>الرحلة 1</v>
+      </c>
+      <c r="F6" t="str">
+        <v>C1</v>
+      </c>
+      <c r="G6" t="str">
+        <v>UNICEF</v>
+      </c>
+      <c r="H6" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٤٤:١٦ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T15:48:01.885Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -558,9 +558,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٤٤:١٦ م</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v/>
+      </c>
+      <c r="B7" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C7" t="str">
+        <v>22</v>
+      </c>
+      <c r="D7" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E7" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="F7" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G7" t="str">
+        <v>WCK</v>
+      </c>
+      <c r="H7" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٤٨:٠١ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T15:49:46.439Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -584,9 +584,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٤٨:٠١ م</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v/>
+      </c>
+      <c r="B8" t="str">
+        <v xml:space="preserve">حسن </v>
+      </c>
+      <c r="C8" t="str">
+        <v>23</v>
+      </c>
+      <c r="D8" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E8" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="F8" t="str">
+        <v>C5</v>
+      </c>
+      <c r="G8" t="str">
+        <v>UNDP</v>
+      </c>
+      <c r="H8" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٤٩:٤٦ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T15:51:05.645Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -610,9 +610,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٤٩:٤٦ م</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v/>
+      </c>
+      <c r="B9" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C9" t="str">
+        <v>23</v>
+      </c>
+      <c r="D9" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E9" t="str">
+        <v>الرحلة 1</v>
+      </c>
+      <c r="F9" t="str">
+        <v>C1</v>
+      </c>
+      <c r="G9" t="str">
+        <v>UNICEF</v>
+      </c>
+      <c r="H9" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٥١:٠٥ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T15:54:17.635Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -636,9 +636,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٥١:٠٥ م</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v/>
+      </c>
+      <c r="B10" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C10" t="str">
+        <v>2323</v>
+      </c>
+      <c r="D10" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E10" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F10" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G10" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H10" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٥٤:١٧ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T15:55:54.591Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -662,9 +662,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٥٤:١٧ م</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v/>
+      </c>
+      <c r="B11" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C11" t="str">
+        <v>23</v>
+      </c>
+      <c r="D11" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E11" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="F11" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G11" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H11" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٥٥:٥٤ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T15:56:56.456Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -688,9 +688,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٥٥:٥٤ م</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v/>
+      </c>
+      <c r="B12" t="str">
+        <v>محمود</v>
+      </c>
+      <c r="C12" t="str">
+        <v>23</v>
+      </c>
+      <c r="D12" t="str">
+        <v>النصر</v>
+      </c>
+      <c r="E12" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F12" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G12" t="str">
+        <v>IDRF</v>
+      </c>
+      <c r="H12" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٥٦:٥٦ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T16:35:01.253Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -480,9 +480,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٦:٥٧:٥٨ م</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v/>
+      </c>
+      <c r="B4" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C4" t="str">
+        <v>2000</v>
+      </c>
+      <c r="D4" t="str">
+        <v>الكويتي</v>
+      </c>
+      <c r="E4" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F4" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G4" t="str">
+        <v>UNDP</v>
+      </c>
+      <c r="H4" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٧:٣٥:٠١ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T16:36:50.762Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -506,9 +506,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٧:٣٥:٠١ م</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v/>
+      </c>
+      <c r="B5" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C5" t="str">
+        <v>222</v>
+      </c>
+      <c r="D5" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E5" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F5" t="str">
+        <v>C1</v>
+      </c>
+      <c r="G5" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H5" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٧:٣٦:٥٠ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 3 rows at 2025-05-01T16:38:04.439Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -532,9 +532,87 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٧:٣٦:٥٠ م</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v/>
+      </c>
+      <c r="B6" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C6" t="str">
+        <v>22</v>
+      </c>
+      <c r="D6" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E6" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F6" t="str">
+        <v>C1</v>
+      </c>
+      <c r="G6" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H6" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٧:٣٨:٠٤ م</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v/>
+      </c>
+      <c r="B7" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C7" t="str">
+        <v>22</v>
+      </c>
+      <c r="D7" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E7" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F7" t="str">
+        <v>C1</v>
+      </c>
+      <c r="G7" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H7" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٧:٣٨:٠٤ م</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v/>
+      </c>
+      <c r="B8" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="C8" t="str">
+        <v>33</v>
+      </c>
+      <c r="D8" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E8" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F8" t="str">
+        <v>C1</v>
+      </c>
+      <c r="G8" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H8" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٧:٣٨:٠٤ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T16:40:01.783Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -610,9 +610,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٧:٣٨:٠٤ م</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v/>
+      </c>
+      <c r="B9" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C9" t="str">
+        <v>222</v>
+      </c>
+      <c r="D9" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E9" t="str">
+        <v>الرحلة 1</v>
+      </c>
+      <c r="F9" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G9" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H9" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٧:٤٠:٠١ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T16:41:35.819Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -636,9 +636,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٧:٤٠:٠١ م</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v/>
+      </c>
+      <c r="B10" t="str">
+        <v>محمود</v>
+      </c>
+      <c r="C10" t="str">
+        <v>222</v>
+      </c>
+      <c r="D10" t="str">
+        <v>النصر</v>
+      </c>
+      <c r="E10" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="F10" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G10" t="str">
+        <v>ABC</v>
+      </c>
+      <c r="H10" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٧:٤١:٣٥ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-01T16:44:30.719Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-01.xlsx
+++ b/Database/Report-2025-05-01.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -662,9 +662,35 @@
         <v>٠١‏/٠٥‏/٢٠٢٥ ٠٧:٤١:٣٥ م</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v/>
+      </c>
+      <c r="B11" t="str">
+        <v>محمود</v>
+      </c>
+      <c r="C11" t="str">
+        <v>2323</v>
+      </c>
+      <c r="D11" t="str">
+        <v>النصر</v>
+      </c>
+      <c r="E11" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="F11" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G11" t="str">
+        <v>ABC</v>
+      </c>
+      <c r="H11" t="str">
+        <v>٠١‏/٠٥‏/٢٠٢٥ ٠٧:٤٤:٣٠ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>